<commit_message>
updated a few variable references and added column names to final excel output
</commit_message>
<xml_diff>
--- a/weights.xlsx
+++ b/weights.xlsx
@@ -12,7 +12,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
   <si>
     <t xml:space="preserve">AMZN</t>
   </si>
@@ -21,6 +27,51 @@
   </si>
   <si>
     <t xml:space="preserve">INTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CACI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPLX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO</t>
   </si>
 </sst>
 </file>
@@ -356,19 +407,153 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2"/>
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.285744577706335</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3"/>
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.194255422293665</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0500000000000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0100000000000006</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.0100000000000001</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.0100000000000002</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.00999999999999994</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.00999999999999989</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.00999999999999952</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0100000000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0100000000000002</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change stock price data to go back 5 years
</commit_message>
<xml_diff>
--- a/weights.xlsx
+++ b/weights.xlsx
@@ -455,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00500000000000001</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0500000000000001</v>
+        <v>0.0500000000000004</v>
       </c>
     </row>
     <row r="4">
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0499999999999999</v>
+        <v>0.0499999999999998</v>
       </c>
     </row>
     <row r="5">
@@ -479,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00500000000000004</v>
+        <v>0.00500000000000005</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00499999999999996</v>
+        <v>0.0150000000000016</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00500000000000014</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="8">
@@ -503,7 +503,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.00500000000000006</v>
+        <v>0.00499999999999982</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00500000000000007</v>
+        <v>0.00500000000000028</v>
       </c>
     </row>
     <row r="10">
@@ -519,7 +519,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0500000000000004</v>
+        <v>0.0499999999999994</v>
       </c>
     </row>
     <row r="11">
@@ -527,7 +527,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00499999999999996</v>
+        <v>0.00500000000000009</v>
       </c>
     </row>
     <row r="12">
@@ -535,7 +535,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>0.00499999999999997</v>
+        <v>0.00500000000000002</v>
       </c>
     </row>
     <row r="13">
@@ -543,7 +543,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0500000000000001</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14">
@@ -551,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0499999999999998</v>
+        <v>0.0500000000000004</v>
       </c>
     </row>
     <row r="15">
@@ -559,7 +559,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0500000000000003</v>
+        <v>0.0499999999999995</v>
       </c>
     </row>
     <row r="16">
@@ -567,7 +567,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>0.00499999999999987</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="17">
@@ -575,7 +575,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>0.00499999999999998</v>
+        <v>0.00500000000000003</v>
       </c>
     </row>
     <row r="18">
@@ -591,7 +591,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0499999999999999</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="20">
@@ -599,7 +599,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>0.00499999999999929</v>
+        <v>0.00500000000000001</v>
       </c>
     </row>
     <row r="21">
@@ -607,7 +607,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0499999999999993</v>
+        <v>0.0500000000000003</v>
       </c>
     </row>
     <row r="22">
@@ -615,7 +615,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>0.00500000000000001</v>
+        <v>0.0500000000000001</v>
       </c>
     </row>
     <row r="23">
@@ -623,7 +623,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="24">
@@ -631,7 +631,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>0.005</v>
+        <v>0.00500000000000003</v>
       </c>
     </row>
     <row r="25">
@@ -647,7 +647,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0500000000000001</v>
+        <v>0.0500000000000004</v>
       </c>
     </row>
     <row r="27">
@@ -655,7 +655,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>0.00499999999999993</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="28">
@@ -663,7 +663,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>0.00499999999999974</v>
+        <v>0.00500000000000014</v>
       </c>
     </row>
     <row r="29">
@@ -671,7 +671,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>0.00499999999999997</v>
+        <v>0.00500000000000002</v>
       </c>
     </row>
     <row r="30">
@@ -679,7 +679,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>0.15</v>
+        <v>0.149999999999998</v>
       </c>
     </row>
     <row r="31">
@@ -687,7 +687,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0499999999999999</v>
+        <v>0.0499999999999998</v>
       </c>
     </row>
     <row r="32">
@@ -695,7 +695,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>0.255000000000001</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>